<commit_message>
more scans and weights
</commit_message>
<xml_diff>
--- a/CG_SLA.xlsx
+++ b/CG_SLA.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$253</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="231">
   <si>
     <t>IND</t>
   </si>
@@ -69,12 +69,6 @@
     <t>BETPOP_HF_5_2</t>
   </si>
   <si>
-    <t>ALNINC_HF_09_1</t>
-  </si>
-  <si>
-    <t>ALNINC_HF_09_2</t>
-  </si>
-  <si>
     <t>BETALL_SH_2_1</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>BETPOP_GR_3_2</t>
   </si>
   <si>
-    <t>BETPOP_GR_5</t>
-  </si>
-  <si>
     <t>BETALL_SH_9_1</t>
   </si>
   <si>
@@ -174,12 +165,6 @@
     <t>ALNINC_GR_1_2</t>
   </si>
   <si>
-    <t>ALNINC_SH_06_1</t>
-  </si>
-  <si>
-    <t>ALNINC_SH_06_2</t>
-  </si>
-  <si>
     <t>ALNINC_GR_8B_1</t>
   </si>
   <si>
@@ -237,9 +222,6 @@
     <t>VIBCAS_WM_9B_1</t>
   </si>
   <si>
-    <t>VIBCAS_WM_9B-2</t>
-  </si>
-  <si>
     <t>SPITOM_HF_13_1</t>
   </si>
   <si>
@@ -468,22 +450,271 @@
     <t>BETPAP_GR_9_2</t>
   </si>
   <si>
-    <t>ALNINC_SH_08_1</t>
-  </si>
-  <si>
-    <t>ALNINC_SH_08_2</t>
-  </si>
-  <si>
-    <t>BETALL_SH_05_1</t>
-  </si>
-  <si>
-    <t>BETALL_SH_05_2</t>
-  </si>
-  <si>
     <t>BETALL_SH_4B_1</t>
   </si>
   <si>
     <t>BETALL_SH_4B_2</t>
+  </si>
+  <si>
+    <t>BETALL_SH_4A_1</t>
+  </si>
+  <si>
+    <t>BETALL_SH_4A_2</t>
+  </si>
+  <si>
+    <t>ALNINC_HF_9_2</t>
+  </si>
+  <si>
+    <t>ALNINC_HF_9_1</t>
+  </si>
+  <si>
+    <t>BETPOP_GR_5_1</t>
+  </si>
+  <si>
+    <t>BETPOP_GR_5_2</t>
+  </si>
+  <si>
+    <t>ALNINC_SH_6_1</t>
+  </si>
+  <si>
+    <t>ALNINC_SH_6_2</t>
+  </si>
+  <si>
+    <t>VIBCAS_WM_9B_2</t>
+  </si>
+  <si>
+    <t>ALNINC_SH_8_1</t>
+  </si>
+  <si>
+    <t>ALNINC_SH_8_2</t>
+  </si>
+  <si>
+    <t>BETALL_WM_8_1</t>
+  </si>
+  <si>
+    <t>BETALL_WM_8_2</t>
+  </si>
+  <si>
+    <t>BETPOP_HF_4_1</t>
+  </si>
+  <si>
+    <t>BETPOP_HF_4_2</t>
+  </si>
+  <si>
+    <t>VIBCAS_SH_5_1</t>
+  </si>
+  <si>
+    <t>VIBCAS_SH_5_2</t>
+  </si>
+  <si>
+    <t>VIBCAS_GR_10_1</t>
+  </si>
+  <si>
+    <t>VIBCAS_GR_10_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_9A_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_9B_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_9B_2</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_5_1</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_5_2</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5E_1</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5E_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8D_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8D_2</t>
+  </si>
+  <si>
+    <t>SPIALB_WM_2B_1</t>
+  </si>
+  <si>
+    <t>SPIALB_WM_2B_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_1B_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_1B_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_9A_2</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_2_1</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_2_2</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_1_1</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_1_2</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5B_1</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5B_2</t>
+  </si>
+  <si>
+    <t>SPIALB_WM_2A_1</t>
+  </si>
+  <si>
+    <t>SPIALB_WM_2A_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_2A_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_2A_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8B_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8B_2</t>
+  </si>
+  <si>
+    <t>SPITOM_SH_99_1</t>
+  </si>
+  <si>
+    <t>SPITOM_SH_99_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8A_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8A_2</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_4_1</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_4_2</t>
+  </si>
+  <si>
+    <t>SPITOM_SH_9_1</t>
+  </si>
+  <si>
+    <t>SPITOM_SH_9_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_1A_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_1A_2</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5C_1</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5C_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_8_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_8_2</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_15_1</t>
+  </si>
+  <si>
+    <t>AROMEL_WM_15_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_4A_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_4A_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_7_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_7_2</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_7_1</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_7_2</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_4B_1</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_4B_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8C_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_GR_8C_2</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_8_1</t>
+  </si>
+  <si>
+    <t>SPIALB_HF_8_2</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5D_1</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5D_2</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_1_1</t>
+  </si>
+  <si>
+    <t>SPIALB_SH_1_2</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_2B_1</t>
+  </si>
+  <si>
+    <t>MYRGAL_SH_2B_2</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5A_1</t>
+  </si>
+  <si>
+    <t>SPITOM_WM_5A_2</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_12_1</t>
+  </si>
+  <si>
+    <t>SPIALB_GR_12_2</t>
+  </si>
+  <si>
+    <t>VIBCAS_GR_9_1</t>
+  </si>
+  <si>
+    <t>VIBCAS_GR_9_2</t>
+  </si>
+  <si>
+    <t>VIBCAS_SH_1_1</t>
+  </si>
+  <si>
+    <t>VIBCAS_SH_1_2</t>
   </si>
 </sst>
 </file>
@@ -888,13 +1119,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C160" sqref="C160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -913,7 +1150,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1">
@@ -1006,7 +1243,7 @@
     </row>
     <row r="10" spans="1:6" hidden="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1017,7 +1254,7 @@
     </row>
     <row r="11" spans="1:6" hidden="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1028,7 +1265,7 @@
     </row>
     <row r="12" spans="1:6" hidden="1">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -1039,7 +1276,7 @@
     </row>
     <row r="13" spans="1:6" hidden="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1050,7 +1287,7 @@
     </row>
     <row r="14" spans="1:6" hidden="1">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -1061,7 +1298,7 @@
     </row>
     <row r="15" spans="1:6" hidden="1">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -1072,7 +1309,7 @@
     </row>
     <row r="16" spans="1:6" hidden="1">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1083,7 +1320,7 @@
     </row>
     <row r="17" spans="1:6" hidden="1">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1094,7 +1331,7 @@
     </row>
     <row r="18" spans="1:6" hidden="1">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -1105,7 +1342,7 @@
     </row>
     <row r="19" spans="1:6" hidden="1">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -1116,7 +1353,7 @@
     </row>
     <row r="20" spans="1:6" hidden="1">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1127,7 +1364,7 @@
     </row>
     <row r="21" spans="1:6" hidden="1">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1138,7 +1375,7 @@
     </row>
     <row r="22" spans="1:6" hidden="1">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -1149,7 +1386,7 @@
     </row>
     <row r="23" spans="1:6" hidden="1">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1160,7 +1397,7 @@
     </row>
     <row r="24" spans="1:6" hidden="1">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -1171,7 +1408,7 @@
     </row>
     <row r="25" spans="1:6" hidden="1">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -1182,7 +1419,7 @@
     </row>
     <row r="26" spans="1:6" hidden="1">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -1193,7 +1430,7 @@
     </row>
     <row r="27" spans="1:6" hidden="1">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -1204,7 +1441,7 @@
     </row>
     <row r="28" spans="1:6" hidden="1">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1215,7 +1452,7 @@
     </row>
     <row r="29" spans="1:6" hidden="1">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="B29">
         <v>6</v>
@@ -1226,7 +1463,7 @@
     </row>
     <row r="30" spans="1:6" hidden="1">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>6</v>
@@ -1237,7 +1474,7 @@
     </row>
     <row r="31" spans="1:6" hidden="1">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -1248,7 +1485,7 @@
     </row>
     <row r="32" spans="1:6" hidden="1">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>6</v>
@@ -1257,12 +1494,12 @@
         <v>0.88519999999999999</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -1271,12 +1508,12 @@
         <v>0.85199999999999998</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -1285,12 +1522,12 @@
         <v>0.48349999999999999</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -1299,12 +1536,12 @@
         <v>0.81369999999999998</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1315,7 +1552,7 @@
     </row>
     <row r="37" spans="1:6" hidden="1">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>5</v>
@@ -1348,7 +1585,7 @@
     </row>
     <row r="40" spans="1:6" hidden="1">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -1359,7 +1596,7 @@
     </row>
     <row r="41" spans="1:6" hidden="1">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -1370,7 +1607,7 @@
     </row>
     <row r="42" spans="1:6" hidden="1">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>5</v>
@@ -1381,7 +1618,7 @@
     </row>
     <row r="43" spans="1:6" hidden="1">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -1392,7 +1629,7 @@
     </row>
     <row r="44" spans="1:6" hidden="1">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -1403,7 +1640,7 @@
     </row>
     <row r="45" spans="1:6" hidden="1">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>5</v>
@@ -1414,7 +1651,7 @@
     </row>
     <row r="46" spans="1:6" hidden="1">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -1425,7 +1662,7 @@
     </row>
     <row r="47" spans="1:6" hidden="1">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -1436,7 +1673,7 @@
     </row>
     <row r="48" spans="1:6" hidden="1">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="B48">
         <v>5</v>
@@ -1447,7 +1684,7 @@
     </row>
     <row r="49" spans="1:3" hidden="1">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -1458,7 +1695,7 @@
     </row>
     <row r="50" spans="1:3" hidden="1">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>5</v>
@@ -1469,7 +1706,7 @@
     </row>
     <row r="51" spans="1:3" hidden="1">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -1480,7 +1717,7 @@
     </row>
     <row r="52" spans="1:3" hidden="1">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -1491,7 +1728,7 @@
     </row>
     <row r="53" spans="1:3" hidden="1">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -1502,7 +1739,7 @@
     </row>
     <row r="54" spans="1:3" hidden="1">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -1513,7 +1750,7 @@
     </row>
     <row r="55" spans="1:3" hidden="1">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -1524,7 +1761,7 @@
     </row>
     <row r="56" spans="1:3" hidden="1">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -1535,7 +1772,7 @@
     </row>
     <row r="57" spans="1:3" hidden="1">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -1546,7 +1783,7 @@
     </row>
     <row r="58" spans="1:3" hidden="1">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -1557,7 +1794,7 @@
     </row>
     <row r="59" spans="1:3" hidden="1">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -1568,7 +1805,7 @@
     </row>
     <row r="60" spans="1:3" hidden="1">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B60">
         <v>5</v>
@@ -1579,7 +1816,7 @@
     </row>
     <row r="61" spans="1:3" hidden="1">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -1590,7 +1827,7 @@
     </row>
     <row r="62" spans="1:3" hidden="1">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B62">
         <v>5</v>
@@ -1601,7 +1838,7 @@
     </row>
     <row r="63" spans="1:3" hidden="1">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -1610,9 +1847,9 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" hidden="1">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -1621,9 +1858,9 @@
         <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" hidden="1">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -1632,9 +1869,9 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" hidden="1">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -1643,9 +1880,9 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" hidden="1">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -1654,9 +1891,9 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" hidden="1">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -1665,9 +1902,9 @@
         <v>5.8900000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" hidden="1">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -1676,9 +1913,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" hidden="1">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -1687,9 +1924,9 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" hidden="1">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -1698,9 +1935,9 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" hidden="1">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -1709,9 +1946,9 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" hidden="1">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -1720,9 +1957,9 @@
         <v>4.53E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" hidden="1">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -1731,9 +1968,9 @@
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" hidden="1">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -1742,9 +1979,9 @@
         <v>7.6399999999999996E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" hidden="1">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -1753,9 +1990,9 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" hidden="1">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B77">
         <v>8</v>
@@ -1764,9 +2001,9 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" hidden="1">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B78">
         <v>8</v>
@@ -1775,9 +2012,9 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" hidden="1">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B79">
         <v>8</v>
@@ -1786,9 +2023,9 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" hidden="1">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B80">
         <v>8</v>
@@ -1797,9 +2034,9 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" hidden="1">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B81">
         <v>8</v>
@@ -1808,9 +2045,9 @@
         <v>4.2099999999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" hidden="1">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>8</v>
@@ -1819,9 +2056,9 @@
         <v>7.1800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" hidden="1">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -1830,9 +2067,9 @@
         <v>6.4600000000000005E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" hidden="1">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <v>8</v>
@@ -1841,9 +2078,9 @@
         <v>6.9699999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" hidden="1">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <v>8</v>
@@ -1852,9 +2089,9 @@
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" hidden="1">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B86">
         <v>8</v>
@@ -1863,9 +2100,9 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" hidden="1">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B87">
         <v>8</v>
@@ -1874,9 +2111,9 @@
         <v>6.8199999999999997E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" hidden="1">
       <c r="A88" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B88">
         <v>8</v>
@@ -1885,9 +2122,9 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" hidden="1">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B89">
         <v>8</v>
@@ -1896,9 +2133,9 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" hidden="1">
       <c r="A90" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B90">
         <v>8</v>
@@ -1907,9 +2144,9 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" hidden="1">
       <c r="A91" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B91">
         <v>8</v>
@@ -1918,9 +2155,9 @@
         <v>3.2300000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" hidden="1">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B92">
         <v>8</v>
@@ -1929,9 +2166,9 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" hidden="1">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B93">
         <v>8</v>
@@ -1940,9 +2177,9 @@
         <v>7.3300000000000004E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" hidden="1">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B94">
         <v>8</v>
@@ -1951,9 +2188,9 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" hidden="1">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B95">
         <v>8</v>
@@ -1962,9 +2199,9 @@
         <v>6.8699999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" hidden="1">
       <c r="A96" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -1973,9 +2210,9 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1">
       <c r="A97" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B97">
         <v>8</v>
@@ -1984,9 +2221,9 @@
         <v>3.9600000000000003E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B98">
         <v>8</v>
@@ -1995,9 +2232,9 @@
         <v>6.54E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B99">
         <v>8</v>
@@ -2006,9 +2243,9 @@
         <v>6.93E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B100">
         <v>8</v>
@@ -2017,9 +2254,9 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B101">
         <v>8</v>
@@ -2028,9 +2265,9 @@
         <v>0.52239999999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B102">
         <v>8</v>
@@ -2039,9 +2276,9 @@
         <v>6.4699999999999994E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" hidden="1">
       <c r="A103" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B103">
         <v>8</v>
@@ -2050,9 +2287,9 @@
         <v>7.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" hidden="1">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B104">
         <v>8</v>
@@ -2061,9 +2298,9 @@
         <v>1.9099999999999999E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" hidden="1">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B105">
         <v>8</v>
@@ -2072,9 +2309,9 @@
         <v>3.6200000000000003E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B106">
         <v>8</v>
@@ -2083,9 +2320,9 @@
         <v>5.16E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1">
       <c r="A107" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B107">
         <v>8</v>
@@ -2094,9 +2331,9 @@
         <v>5.5300000000000002E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B108">
         <v>8</v>
@@ -2105,9 +2342,9 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B109">
         <v>8</v>
@@ -2116,9 +2353,9 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B110">
         <v>8</v>
@@ -2127,9 +2364,9 @@
         <v>9.7600000000000006E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B111">
         <v>8</v>
@@ -2138,9 +2375,9 @@
         <v>6.0900000000000003E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B112">
         <v>8</v>
@@ -2149,9 +2386,9 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" hidden="1">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B113">
         <v>8</v>
@@ -2160,9 +2397,9 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" hidden="1">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B114">
         <v>8</v>
@@ -2171,9 +2408,9 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" hidden="1">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B115">
         <v>8</v>
@@ -2182,9 +2419,9 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" hidden="1">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B116">
         <v>8</v>
@@ -2193,9 +2430,9 @@
         <v>0.18260000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" hidden="1">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B117">
         <v>8</v>
@@ -2204,9 +2441,9 @@
         <v>0.19620000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" hidden="1">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B118">
         <v>8</v>
@@ -2215,9 +2452,9 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" hidden="1">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B119">
         <v>8</v>
@@ -2226,9 +2463,9 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" hidden="1">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B120">
         <v>8</v>
@@ -2237,9 +2474,9 @@
         <v>3.2199999999999999E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" hidden="1">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B121">
         <v>8</v>
@@ -2248,9 +2485,9 @@
         <v>6.0600000000000001E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" hidden="1">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B122">
         <v>8</v>
@@ -2259,9 +2496,9 @@
         <v>8.0799999999999997E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" hidden="1">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B123">
         <v>8</v>
@@ -2270,9 +2507,9 @@
         <v>9.5699999999999993E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" hidden="1">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B124">
         <v>8</v>
@@ -2281,9 +2518,9 @@
         <v>5.4699999999999999E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" hidden="1">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B125">
         <v>8</v>
@@ -2292,9 +2529,9 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" hidden="1">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B126">
         <v>8</v>
@@ -2303,9 +2540,9 @@
         <v>0.1075</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" hidden="1">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B127">
         <v>8</v>
@@ -2314,9 +2551,9 @@
         <v>7.7899999999999997E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" hidden="1">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B128">
         <v>8</v>
@@ -2325,9 +2562,9 @@
         <v>6.9940000000000002E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" hidden="1">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B129">
         <v>8</v>
@@ -2336,9 +2573,9 @@
         <v>8.4570000000000006E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" hidden="1">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B130">
         <v>8</v>
@@ -2347,9 +2584,9 @@
         <v>0.52029999999999998</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" hidden="1">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B131">
         <v>8</v>
@@ -2358,9 +2595,9 @@
         <v>0.62329999999999997</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" hidden="1">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B132">
         <v>8</v>
@@ -2369,9 +2606,9 @@
         <v>2.53E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" hidden="1">
       <c r="A133" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B133">
         <v>8</v>
@@ -2380,9 +2617,9 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" hidden="1">
       <c r="A134" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B134">
         <v>8</v>
@@ -2391,9 +2628,9 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" hidden="1">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B135">
         <v>8</v>
@@ -2402,9 +2639,9 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" hidden="1">
       <c r="A136" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B136">
         <v>8</v>
@@ -2413,9 +2650,9 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" hidden="1">
       <c r="A137" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B137">
         <v>8</v>
@@ -2424,9 +2661,9 @@
         <v>0.308</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" hidden="1">
       <c r="A138" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B138">
         <v>8</v>
@@ -2435,9 +2672,9 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" hidden="1">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B139">
         <v>8</v>
@@ -2446,9 +2683,9 @@
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" hidden="1">
       <c r="A140" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B140">
         <v>8</v>
@@ -2457,9 +2694,9 @@
         <v>7.1400000000000005E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" hidden="1">
       <c r="A141" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B141">
         <v>8</v>
@@ -2468,9 +2705,9 @@
         <v>6.7339999999999997E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" hidden="1">
       <c r="A142" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B142">
         <v>8</v>
@@ -2479,9 +2716,9 @@
         <v>0.61560000000000004</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" hidden="1">
       <c r="A143" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B143">
         <v>8</v>
@@ -2490,9 +2727,9 @@
         <v>0.5121</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" hidden="1">
       <c r="A144" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B144">
         <v>8</v>
@@ -2501,9 +2738,9 @@
         <v>0.73599999999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" hidden="1">
       <c r="A145" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B145">
         <v>8</v>
@@ -2514,7 +2751,7 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B146">
         <v>9</v>
@@ -2525,7 +2762,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B147">
         <v>9</v>
@@ -2558,7 +2795,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B150">
         <v>9</v>
@@ -2569,7 +2806,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B151">
         <v>9</v>
@@ -2580,7 +2817,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="B152">
         <v>9</v>
@@ -2591,7 +2828,7 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="B153">
         <v>9</v>
@@ -2602,7 +2839,7 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B154">
         <v>9</v>
@@ -2613,7 +2850,7 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B155">
         <v>9</v>
@@ -2624,7 +2861,7 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
       <c r="B156">
         <v>9</v>
@@ -2635,7 +2872,7 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>151</v>
+        <v>18</v>
       </c>
       <c r="B157">
         <v>9</v>
@@ -2646,7 +2883,7 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B158">
         <v>9</v>
@@ -2657,7 +2894,7 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B159">
         <v>9</v>
@@ -2666,11 +2903,1045 @@
         <v>0.189</v>
       </c>
     </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>144</v>
+      </c>
+      <c r="B160">
+        <v>9</v>
+      </c>
+      <c r="C160">
+        <v>0.31619999999999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>145</v>
+      </c>
+      <c r="B161">
+        <v>9</v>
+      </c>
+      <c r="C161">
+        <v>0.32763999999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>147</v>
+      </c>
+      <c r="B162">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <v>0.45304</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>146</v>
+      </c>
+      <c r="B163">
+        <v>9</v>
+      </c>
+      <c r="C163">
+        <v>0.48233999999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>157</v>
+      </c>
+      <c r="B164">
+        <v>9</v>
+      </c>
+      <c r="C164">
+        <v>0.21459</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>158</v>
+      </c>
+      <c r="B165">
+        <v>9</v>
+      </c>
+      <c r="C165">
+        <v>0.25752999999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" hidden="1">
+      <c r="A166" t="s">
+        <v>159</v>
+      </c>
+      <c r="B166">
+        <v>4</v>
+      </c>
+      <c r="C166">
+        <v>0.49186000000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" hidden="1">
+      <c r="A167" t="s">
+        <v>160</v>
+      </c>
+      <c r="B167">
+        <v>4</v>
+      </c>
+      <c r="C167">
+        <v>0.92889999999999995</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" hidden="1">
+      <c r="A168" t="s">
+        <v>161</v>
+      </c>
+      <c r="B168">
+        <v>4</v>
+      </c>
+      <c r="C168">
+        <v>0.37663999999999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" hidden="1">
+      <c r="A169" t="s">
+        <v>162</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+      <c r="C169">
+        <v>0.71209999999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" hidden="1">
+      <c r="A170" t="s">
+        <v>164</v>
+      </c>
+      <c r="B170">
+        <v>4</v>
+      </c>
+      <c r="C170">
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" hidden="1">
+      <c r="A171" t="s">
+        <v>165</v>
+      </c>
+      <c r="B171">
+        <v>4</v>
+      </c>
+      <c r="C171">
+        <v>7.6609999999999998E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" hidden="1">
+      <c r="A172" t="s">
+        <v>166</v>
+      </c>
+      <c r="B172">
+        <v>4</v>
+      </c>
+      <c r="C172">
+        <v>0.10367999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" hidden="1">
+      <c r="A173" t="s">
+        <v>167</v>
+      </c>
+      <c r="B173">
+        <v>4</v>
+      </c>
+      <c r="C173">
+        <v>0.15343999999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" hidden="1">
+      <c r="A174" t="s">
+        <v>168</v>
+      </c>
+      <c r="B174">
+        <v>4</v>
+      </c>
+      <c r="C174">
+        <v>3.5360000000000003E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" hidden="1">
+      <c r="A175" t="s">
+        <v>169</v>
+      </c>
+      <c r="B175">
+        <v>4</v>
+      </c>
+      <c r="C175">
+        <v>4.2880000000000001E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" hidden="1">
+      <c r="A176" t="s">
+        <v>84</v>
+      </c>
+      <c r="B176">
+        <v>4</v>
+      </c>
+      <c r="C176">
+        <v>7.5230000000000005E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" hidden="1">
+      <c r="A177" t="s">
+        <v>85</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+      <c r="C177">
+        <v>7.4310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" hidden="1">
+      <c r="A178" t="s">
+        <v>170</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178">
+        <v>6.2710000000000002E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" hidden="1">
+      <c r="A179" t="s">
+        <v>171</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+      <c r="C179">
+        <v>8.43E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" hidden="1">
+      <c r="A180" t="s">
+        <v>172</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180">
+        <v>4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" hidden="1">
+      <c r="A181" t="s">
+        <v>173</v>
+      </c>
+      <c r="B181">
+        <v>4</v>
+      </c>
+      <c r="C181">
+        <v>5.3499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" hidden="1">
+      <c r="A182" t="s">
+        <v>174</v>
+      </c>
+      <c r="B182">
+        <v>4</v>
+      </c>
+      <c r="C182">
+        <v>5.8099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" hidden="1">
+      <c r="A183" t="s">
+        <v>175</v>
+      </c>
+      <c r="B183">
+        <v>4</v>
+      </c>
+      <c r="C183">
+        <v>6.5500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" hidden="1">
+      <c r="A184" t="s">
+        <v>128</v>
+      </c>
+      <c r="B184">
+        <v>4</v>
+      </c>
+      <c r="C184">
+        <v>5.9799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" hidden="1">
+      <c r="A185" t="s">
+        <v>129</v>
+      </c>
+      <c r="B185">
+        <v>4</v>
+      </c>
+      <c r="C185">
+        <v>7.8899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" hidden="1">
+      <c r="A186" t="s">
+        <v>163</v>
+      </c>
+      <c r="B186">
+        <v>4</v>
+      </c>
+      <c r="C186">
+        <v>5.8400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" hidden="1">
+      <c r="A187" t="s">
+        <v>176</v>
+      </c>
+      <c r="B187">
+        <v>4</v>
+      </c>
+      <c r="C187">
+        <v>7.0599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" hidden="1">
+      <c r="A188" t="s">
+        <v>177</v>
+      </c>
+      <c r="B188">
+        <v>4</v>
+      </c>
+      <c r="C188">
+        <v>0.22586999999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" hidden="1">
+      <c r="A189" t="s">
+        <v>178</v>
+      </c>
+      <c r="B189">
+        <v>4</v>
+      </c>
+      <c r="C189">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" hidden="1">
+      <c r="A190" t="s">
+        <v>179</v>
+      </c>
+      <c r="B190">
+        <v>4</v>
+      </c>
+      <c r="C190">
+        <v>8.9149999999999993E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" hidden="1">
+      <c r="A191" t="s">
+        <v>180</v>
+      </c>
+      <c r="B191">
+        <v>4</v>
+      </c>
+      <c r="C191">
+        <v>8.3659999999999998E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" hidden="1">
+      <c r="A192" t="s">
+        <v>181</v>
+      </c>
+      <c r="B192">
+        <v>4</v>
+      </c>
+      <c r="C192">
+        <v>7.7130000000000004E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" hidden="1">
+      <c r="A193" t="s">
+        <v>182</v>
+      </c>
+      <c r="B193">
+        <v>4</v>
+      </c>
+      <c r="C193">
+        <v>8.9370000000000005E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" hidden="1">
+      <c r="A194" t="s">
+        <v>183</v>
+      </c>
+      <c r="B194">
+        <v>4</v>
+      </c>
+      <c r="C194">
+        <v>6.3960000000000003E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" hidden="1">
+      <c r="A195" t="s">
+        <v>184</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+      <c r="C195">
+        <v>8.5180000000000006E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" hidden="1">
+      <c r="A196" t="s">
+        <v>185</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+      <c r="C196">
+        <v>7.3099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" hidden="1">
+      <c r="A197" t="s">
+        <v>186</v>
+      </c>
+      <c r="B197">
+        <v>4</v>
+      </c>
+      <c r="C197">
+        <v>6.2640000000000001E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" hidden="1">
+      <c r="A198" t="s">
+        <v>187</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+      <c r="C198">
+        <v>6.4579999999999999E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" hidden="1">
+      <c r="A199" t="s">
+        <v>188</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+      <c r="C199">
+        <v>6.6769999999999996E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" hidden="1">
+      <c r="A200" t="s">
+        <v>189</v>
+      </c>
+      <c r="B200">
+        <v>4</v>
+      </c>
+      <c r="C200">
+        <v>2.452E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" hidden="1">
+      <c r="A201" t="s">
+        <v>190</v>
+      </c>
+      <c r="B201">
+        <v>4</v>
+      </c>
+      <c r="C201">
+        <v>2.93E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" hidden="1">
+      <c r="A202" t="s">
+        <v>191</v>
+      </c>
+      <c r="B202">
+        <v>4</v>
+      </c>
+      <c r="C202">
+        <v>8.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" hidden="1">
+      <c r="A203" t="s">
+        <v>192</v>
+      </c>
+      <c r="B203">
+        <v>4</v>
+      </c>
+      <c r="C203">
+        <v>8.4599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" hidden="1">
+      <c r="A204" t="s">
+        <v>193</v>
+      </c>
+      <c r="B204">
+        <v>4</v>
+      </c>
+      <c r="C204">
+        <v>2.828E-2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" hidden="1">
+      <c r="A205" t="s">
+        <v>194</v>
+      </c>
+      <c r="B205">
+        <v>4</v>
+      </c>
+      <c r="C205">
+        <v>5.246E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" hidden="1">
+      <c r="A206" t="s">
+        <v>195</v>
+      </c>
+      <c r="B206">
+        <v>4</v>
+      </c>
+      <c r="C206">
+        <v>3.517E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" hidden="1">
+      <c r="A207" t="s">
+        <v>196</v>
+      </c>
+      <c r="B207">
+        <v>4</v>
+      </c>
+      <c r="C207">
+        <v>5.3830000000000003E-2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" hidden="1">
+      <c r="A208" t="s">
+        <v>197</v>
+      </c>
+      <c r="B208">
+        <v>4</v>
+      </c>
+      <c r="C208">
+        <v>6.4130000000000006E-2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" hidden="1">
+      <c r="A209" t="s">
+        <v>198</v>
+      </c>
+      <c r="B209">
+        <v>4</v>
+      </c>
+      <c r="C209">
+        <v>6.1170000000000002E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" hidden="1">
+      <c r="A210" t="s">
+        <v>76</v>
+      </c>
+      <c r="B210">
+        <v>4</v>
+      </c>
+      <c r="C210">
+        <v>6.0229999999999999E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" hidden="1">
+      <c r="A211" t="s">
+        <v>77</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="C211">
+        <v>6.1469999999999997E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" hidden="1">
+      <c r="A212" t="s">
+        <v>132</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+      <c r="C212">
+        <v>0.41488999999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" hidden="1">
+      <c r="A213" t="s">
+        <v>133</v>
+      </c>
+      <c r="B213">
+        <v>4</v>
+      </c>
+      <c r="C213">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" hidden="1">
+      <c r="A214" t="s">
+        <v>199</v>
+      </c>
+      <c r="B214">
+        <v>4</v>
+      </c>
+      <c r="C214">
+        <v>5.5590000000000001E-2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" hidden="1">
+      <c r="A215" t="s">
+        <v>200</v>
+      </c>
+      <c r="B215">
+        <v>4</v>
+      </c>
+      <c r="C215">
+        <v>6.1019999999999998E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" hidden="1">
+      <c r="A216" t="s">
+        <v>201</v>
+      </c>
+      <c r="B216">
+        <v>4</v>
+      </c>
+      <c r="C216">
+        <v>6.0499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" hidden="1">
+      <c r="A217" t="s">
+        <v>202</v>
+      </c>
+      <c r="B217">
+        <v>4</v>
+      </c>
+      <c r="C217">
+        <v>7.2040000000000007E-2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" hidden="1">
+      <c r="A218" t="s">
+        <v>98</v>
+      </c>
+      <c r="B218">
+        <v>4</v>
+      </c>
+      <c r="C218">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" hidden="1">
+      <c r="A219" t="s">
+        <v>99</v>
+      </c>
+      <c r="B219">
+        <v>4</v>
+      </c>
+      <c r="C219">
+        <v>0.79190000000000005</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" hidden="1">
+      <c r="A220" t="s">
+        <v>203</v>
+      </c>
+      <c r="B220">
+        <v>4</v>
+      </c>
+      <c r="C220">
+        <v>0.13757</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" hidden="1">
+      <c r="A221" t="s">
+        <v>204</v>
+      </c>
+      <c r="B221">
+        <v>4</v>
+      </c>
+      <c r="C221">
+        <v>0.13672999999999999</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" hidden="1">
+      <c r="A222" t="s">
+        <v>205</v>
+      </c>
+      <c r="B222">
+        <v>4</v>
+      </c>
+      <c r="C222">
+        <v>6.5030000000000004E-2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" hidden="1">
+      <c r="A223" t="s">
+        <v>206</v>
+      </c>
+      <c r="B223">
+        <v>4</v>
+      </c>
+      <c r="C223">
+        <v>7.7950000000000005E-2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" hidden="1">
+      <c r="A224" t="s">
+        <v>207</v>
+      </c>
+      <c r="B224">
+        <v>4</v>
+      </c>
+      <c r="C224">
+        <v>8.6669999999999997E-2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" hidden="1">
+      <c r="A225" t="s">
+        <v>208</v>
+      </c>
+      <c r="B225">
+        <v>4</v>
+      </c>
+      <c r="C225">
+        <v>9.5200000000000007E-2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" hidden="1">
+      <c r="A226" t="s">
+        <v>116</v>
+      </c>
+      <c r="B226">
+        <v>4</v>
+      </c>
+      <c r="C226">
+        <v>3.2530000000000003E-2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" hidden="1">
+      <c r="A227" t="s">
+        <v>117</v>
+      </c>
+      <c r="B227">
+        <v>4</v>
+      </c>
+      <c r="C227">
+        <v>5.0250000000000003E-2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" hidden="1">
+      <c r="A228" t="s">
+        <v>209</v>
+      </c>
+      <c r="B228">
+        <v>4</v>
+      </c>
+      <c r="C228">
+        <v>6.4630000000000007E-2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" hidden="1">
+      <c r="A229" t="s">
+        <v>210</v>
+      </c>
+      <c r="B229">
+        <v>4</v>
+      </c>
+      <c r="C229">
+        <v>9.9790000000000004E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" hidden="1">
+      <c r="A230" t="s">
+        <v>211</v>
+      </c>
+      <c r="B230">
+        <v>4</v>
+      </c>
+      <c r="C230">
+        <v>4.4339999999999997E-2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" hidden="1">
+      <c r="A231" t="s">
+        <v>212</v>
+      </c>
+      <c r="B231">
+        <v>4</v>
+      </c>
+      <c r="C231">
+        <v>4.598E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" hidden="1">
+      <c r="A232" t="s">
+        <v>70</v>
+      </c>
+      <c r="B232">
+        <v>4</v>
+      </c>
+      <c r="C232">
+        <v>0.56067</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" hidden="1">
+      <c r="A233" t="s">
+        <v>71</v>
+      </c>
+      <c r="B233">
+        <v>4</v>
+      </c>
+      <c r="C233">
+        <v>0.78349999999999997</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" hidden="1">
+      <c r="A234" t="s">
+        <v>100</v>
+      </c>
+      <c r="B234">
+        <v>4</v>
+      </c>
+      <c r="C234">
+        <v>0.10165</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" hidden="1">
+      <c r="A235" t="s">
+        <v>101</v>
+      </c>
+      <c r="B235">
+        <v>4</v>
+      </c>
+      <c r="C235">
+        <v>9.5829999999999999E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" hidden="1">
+      <c r="A236" t="s">
+        <v>213</v>
+      </c>
+      <c r="B236">
+        <v>4</v>
+      </c>
+      <c r="C236">
+        <v>5.457E-2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" hidden="1">
+      <c r="A237" t="s">
+        <v>214</v>
+      </c>
+      <c r="B237">
+        <v>4</v>
+      </c>
+      <c r="C237">
+        <v>9.4490000000000005E-2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" hidden="1">
+      <c r="A238" t="s">
+        <v>215</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+      <c r="C238">
+        <v>8.4070000000000006E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" hidden="1">
+      <c r="A239" t="s">
+        <v>216</v>
+      </c>
+      <c r="B239">
+        <v>4</v>
+      </c>
+      <c r="C239">
+        <v>0.10272000000000001</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" hidden="1">
+      <c r="A240" t="s">
+        <v>217</v>
+      </c>
+      <c r="B240">
+        <v>4</v>
+      </c>
+      <c r="C240">
+        <v>1.8360000000000001E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" hidden="1">
+      <c r="A241" t="s">
+        <v>218</v>
+      </c>
+      <c r="B241">
+        <v>4</v>
+      </c>
+      <c r="C241">
+        <v>3.2649999999999998E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" hidden="1">
+      <c r="A242" t="s">
+        <v>219</v>
+      </c>
+      <c r="B242">
+        <v>4</v>
+      </c>
+      <c r="C242">
+        <v>7.8289999999999998E-2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" hidden="1">
+      <c r="A243" t="s">
+        <v>220</v>
+      </c>
+      <c r="B243">
+        <v>4</v>
+      </c>
+      <c r="C243">
+        <v>7.4079999999999993E-2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" hidden="1">
+      <c r="A244" t="s">
+        <v>221</v>
+      </c>
+      <c r="B244">
+        <v>4</v>
+      </c>
+      <c r="C244">
+        <v>3.2980000000000002E-2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" hidden="1">
+      <c r="A245" t="s">
+        <v>222</v>
+      </c>
+      <c r="B245">
+        <v>4</v>
+      </c>
+      <c r="C245">
+        <v>3.7440000000000001E-2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" hidden="1">
+      <c r="A246" t="s">
+        <v>223</v>
+      </c>
+      <c r="B246">
+        <v>4</v>
+      </c>
+      <c r="C246">
+        <v>0.11504</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" hidden="1">
+      <c r="A247" t="s">
+        <v>224</v>
+      </c>
+      <c r="B247">
+        <v>4</v>
+      </c>
+      <c r="C247">
+        <v>0.19739999999999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" hidden="1">
+      <c r="A248" t="s">
+        <v>225</v>
+      </c>
+      <c r="B248">
+        <v>4</v>
+      </c>
+      <c r="C248">
+        <v>3.1620000000000002E-2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" hidden="1">
+      <c r="A249" t="s">
+        <v>226</v>
+      </c>
+      <c r="B249">
+        <v>4</v>
+      </c>
+      <c r="C249">
+        <v>6.0199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" hidden="1">
+      <c r="A250" t="s">
+        <v>227</v>
+      </c>
+      <c r="B250">
+        <v>4</v>
+      </c>
+      <c r="C250">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" hidden="1">
+      <c r="A251" t="s">
+        <v>228</v>
+      </c>
+      <c r="B251">
+        <v>4</v>
+      </c>
+      <c r="C251">
+        <v>0.69599999999999995</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" hidden="1">
+      <c r="A252" t="s">
+        <v>229</v>
+      </c>
+      <c r="B252">
+        <v>4</v>
+      </c>
+      <c r="C252">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" hidden="1">
+      <c r="A253" t="s">
+        <v>230</v>
+      </c>
+      <c r="B253">
+        <v>4</v>
+      </c>
+      <c r="C253">
+        <v>0.77354999999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F145">
+  <autoFilter ref="A1:F253">
     <filterColumn colId="1">
       <filters>
-        <filter val="8"/>
+        <filter val="9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
updates to pore anatomy
</commit_message>
<xml_diff>
--- a/CG_SLA.xlsx
+++ b/CG_SLA.xlsx
@@ -5,17 +5,19 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/CGtraits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/GitHub/CGtraits/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21960" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="26940" yWindow="1900" windowWidth="21960" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$383</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="341">
   <si>
     <t>IND</t>
   </si>
@@ -966,6 +968,93 @@
   </si>
   <si>
     <t>VIBCAS_WM_10_2</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Pore Anatomy</t>
+  </si>
+  <si>
+    <t>Wood anatomy features</t>
+  </si>
+  <si>
+    <t>International Association of Wood Anatomists IAWA</t>
+  </si>
+  <si>
+    <t>Pore anatomy</t>
+  </si>
+  <si>
+    <t>diffuse-porous</t>
+  </si>
+  <si>
+    <t>ring-porous</t>
+  </si>
+  <si>
+    <t>semi-porous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From insidewood.lib.ncsu.edu - (from Dan Flynn's </t>
+  </si>
+  <si>
+    <t>ACEPEN</t>
+  </si>
+  <si>
+    <t>ACESPI</t>
+  </si>
+  <si>
+    <t>ALNINC</t>
+  </si>
+  <si>
+    <t>AROMEL</t>
+  </si>
+  <si>
+    <t>AMECAN</t>
+  </si>
+  <si>
+    <t>BETALL</t>
+  </si>
+  <si>
+    <t>BETPAP</t>
+  </si>
+  <si>
+    <t>BETPOP</t>
+  </si>
+  <si>
+    <t>DIELON</t>
+  </si>
+  <si>
+    <t>MYRGAL</t>
+  </si>
+  <si>
+    <t>QUEALB</t>
+  </si>
+  <si>
+    <t>QUERUB</t>
+  </si>
+  <si>
+    <t>SAMRAC</t>
+  </si>
+  <si>
+    <t>SORAME</t>
+  </si>
+  <si>
+    <t>SPIALB</t>
+  </si>
+  <si>
+    <t>SPITOM</t>
+  </si>
+  <si>
+    <t>VACMYR</t>
+  </si>
+  <si>
+    <t>VIBCAS</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Serrations</t>
   </si>
 </sst>
 </file>
@@ -1373,14 +1462,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F383"/>
+  <dimension ref="A1:G383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B360" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C382" sqref="C382"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1388,7 +1476,7 @@
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1407,8 +1495,11 @@
       <c r="F1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1510,7 @@
         <v>0.38679999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1430,7 +1521,7 @@
         <v>0.32601999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1441,7 +1532,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1452,7 +1543,7 @@
         <v>0.26169999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1463,7 +1554,7 @@
         <v>8.3799999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1474,7 +1565,7 @@
         <v>7.6600000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1576,7 @@
         <v>0.36170000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1587,7 @@
         <v>0.48370000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>147</v>
       </c>
@@ -1507,7 +1598,7 @@
         <v>0.63829999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>146</v>
       </c>
@@ -1518,7 +1609,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1529,7 +1620,7 @@
         <v>0.70479999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1540,7 +1631,7 @@
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1551,7 +1642,7 @@
         <v>0.51749999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1562,7 +1653,7 @@
         <v>0.3402</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1573,7 +1664,7 @@
         <v>0.55559999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1584,7 +1675,7 @@
         <v>0.75890000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1595,7 +1686,7 @@
         <v>0.26379999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1606,7 +1697,7 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1617,7 +1708,7 @@
         <v>0.34010000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1628,7 +1719,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1639,7 +1730,7 @@
         <v>0.43099999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1650,7 +1741,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1661,7 +1752,7 @@
         <v>0.21690000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1672,7 +1763,7 @@
         <v>0.43340000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1683,7 +1774,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1694,7 +1785,7 @@
         <v>0.43469999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -1705,7 +1796,7 @@
         <v>0.38879999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -1716,7 +1807,7 @@
         <v>0.36480000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1818,7 @@
         <v>0.51639999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1738,7 +1829,7 @@
         <v>0.502</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1766,7 +1857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1780,7 +1871,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1794,7 +1885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1805,7 +1896,7 @@
         <v>1.1559999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1816,7 +1907,7 @@
         <v>1.341</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1827,7 +1918,7 @@
         <v>1.083</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1838,7 +1929,7 @@
         <v>1.135</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1849,7 +1940,7 @@
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1860,7 +1951,7 @@
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -1871,7 +1962,7 @@
         <v>0.17610000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1882,7 +1973,7 @@
         <v>0.1447</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1893,7 +1984,7 @@
         <v>0.50560000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1904,7 +1995,7 @@
         <v>0.38812999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1915,7 +2006,7 @@
         <v>0.73070000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1926,7 +2017,7 @@
         <v>0.99580000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>150</v>
       </c>
@@ -1937,7 +2028,7 @@
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -1948,7 +2039,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1959,7 +2050,7 @@
         <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1970,7 +2061,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1981,7 +2072,7 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1992,7 +2083,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2003,7 +2094,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2014,7 +2105,7 @@
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2025,7 +2116,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -2036,7 +2127,7 @@
         <v>0.17399999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -2047,7 +2138,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -2058,7 +2149,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -2069,7 +2160,7 @@
         <v>0.17699999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -2080,7 +2171,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -2091,7 +2182,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>58</v>
       </c>
@@ -2102,7 +2193,7 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -2113,7 +2204,7 @@
         <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -2124,7 +2215,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>61</v>
       </c>
@@ -2135,7 +2226,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -2146,7 +2237,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -2157,7 +2248,7 @@
         <v>5.8900000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>64</v>
       </c>
@@ -2168,7 +2259,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -2179,7 +2270,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>152</v>
       </c>
@@ -2190,7 +2281,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -2201,7 +2292,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -2212,7 +2303,7 @@
         <v>4.53E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -2223,7 +2314,7 @@
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -2234,7 +2325,7 @@
         <v>7.6399999999999996E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -2245,7 +2336,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -2256,7 +2347,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -2267,7 +2358,7 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -2278,7 +2369,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -2289,7 +2380,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>75</v>
       </c>
@@ -2300,7 +2391,7 @@
         <v>4.2099999999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -2311,7 +2402,7 @@
         <v>7.1800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -2322,7 +2413,7 @@
         <v>6.4600000000000005E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>78</v>
       </c>
@@ -2333,7 +2424,7 @@
         <v>6.9699999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -2344,7 +2435,7 @@
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -2355,7 +2446,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -2366,7 +2457,7 @@
         <v>6.8199999999999997E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>134</v>
       </c>
@@ -2377,7 +2468,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>135</v>
       </c>
@@ -2388,7 +2479,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>137</v>
       </c>
@@ -2399,7 +2490,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>136</v>
       </c>
@@ -2410,7 +2501,7 @@
         <v>3.2300000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>84</v>
       </c>
@@ -2421,7 +2512,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -2432,7 +2523,7 @@
         <v>7.3300000000000004E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>86</v>
       </c>
@@ -2443,7 +2534,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -2454,7 +2545,7 @@
         <v>6.8699999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -2465,7 +2556,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -2476,7 +2567,7 @@
         <v>3.9600000000000003E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>88</v>
       </c>
@@ -2487,7 +2578,7 @@
         <v>6.54E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>89</v>
       </c>
@@ -2498,7 +2589,7 @@
         <v>6.93E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>90</v>
       </c>
@@ -2509,7 +2600,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>91</v>
       </c>
@@ -2520,7 +2611,7 @@
         <v>0.52239999999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>92</v>
       </c>
@@ -2531,7 +2622,7 @@
         <v>6.4699999999999994E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>93</v>
       </c>
@@ -2542,7 +2633,7 @@
         <v>7.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>94</v>
       </c>
@@ -2553,7 +2644,7 @@
         <v>1.9099999999999999E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>95</v>
       </c>
@@ -2564,7 +2655,7 @@
         <v>3.6200000000000003E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>82</v>
       </c>
@@ -2575,7 +2666,7 @@
         <v>5.16E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>83</v>
       </c>
@@ -2586,7 +2677,7 @@
         <v>5.5300000000000002E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>98</v>
       </c>
@@ -2597,7 +2688,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>99</v>
       </c>
@@ -2608,7 +2699,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -2619,7 +2710,7 @@
         <v>9.7600000000000006E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -2630,7 +2721,7 @@
         <v>6.0900000000000003E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>102</v>
       </c>
@@ -2641,7 +2732,7 @@
         <v>0.81599999999999995</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>103</v>
       </c>
@@ -2652,7 +2743,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -2663,7 +2754,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>105</v>
       </c>
@@ -2674,7 +2765,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -2685,7 +2776,7 @@
         <v>0.18260000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>107</v>
       </c>
@@ -2696,7 +2787,7 @@
         <v>0.19620000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -2707,7 +2798,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>109</v>
       </c>
@@ -2718,7 +2809,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>110</v>
       </c>
@@ -2729,7 +2820,7 @@
         <v>3.2199999999999999E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>111</v>
       </c>
@@ -2740,7 +2831,7 @@
         <v>6.0600000000000001E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>112</v>
       </c>
@@ -2751,7 +2842,7 @@
         <v>8.0799999999999997E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>113</v>
       </c>
@@ -2762,7 +2853,7 @@
         <v>9.5699999999999993E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>114</v>
       </c>
@@ -2773,7 +2864,7 @@
         <v>5.4699999999999999E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>115</v>
       </c>
@@ -2784,7 +2875,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>116</v>
       </c>
@@ -2795,7 +2886,7 @@
         <v>0.1075</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>117</v>
       </c>
@@ -2806,7 +2897,7 @@
         <v>7.7899999999999997E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -2817,7 +2908,7 @@
         <v>6.9940000000000002E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>119</v>
       </c>
@@ -2828,7 +2919,7 @@
         <v>8.4570000000000006E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>120</v>
       </c>
@@ -2839,7 +2930,7 @@
         <v>0.52029999999999998</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>121</v>
       </c>
@@ -2850,7 +2941,7 @@
         <v>0.62329999999999997</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -2861,7 +2952,7 @@
         <v>2.53E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -2872,7 +2963,7 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>122</v>
       </c>
@@ -2883,7 +2974,7 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>123</v>
       </c>
@@ -2894,7 +2985,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>124</v>
       </c>
@@ -2905,7 +2996,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>125</v>
       </c>
@@ -2916,7 +3007,7 @@
         <v>0.308</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -2927,7 +3018,7 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -2938,7 +3029,7 @@
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>128</v>
       </c>
@@ -2949,7 +3040,7 @@
         <v>7.1400000000000005E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>129</v>
       </c>
@@ -2960,7 +3051,7 @@
         <v>6.7339999999999997E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>130</v>
       </c>
@@ -2971,7 +3062,7 @@
         <v>0.61560000000000004</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>131</v>
       </c>
@@ -2982,7 +3073,7 @@
         <v>0.5121</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>132</v>
       </c>
@@ -2993,7 +3084,7 @@
         <v>0.73599999999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>133</v>
       </c>
@@ -3004,7 +3095,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -3015,7 +3106,7 @@
         <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>32</v>
       </c>
@@ -3026,7 +3117,7 @@
         <v>0.34849999999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -3037,7 +3128,7 @@
         <v>0.29110000000000003</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -3048,7 +3139,7 @@
         <v>0.39269999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>140</v>
       </c>
@@ -3059,7 +3150,7 @@
         <v>0.91469999999999996</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>141</v>
       </c>
@@ -3070,7 +3161,7 @@
         <v>0.91110000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>155</v>
       </c>
@@ -3081,7 +3172,7 @@
         <v>0.30409999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>156</v>
       </c>
@@ -3092,7 +3183,7 @@
         <v>0.3831</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3103,7 +3194,7 @@
         <v>0.50380000000000003</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3114,7 +3205,7 @@
         <v>0.49509999999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>17</v>
       </c>
@@ -3125,7 +3216,7 @@
         <v>0.62160000000000004</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>18</v>
       </c>
@@ -3136,7 +3227,7 @@
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>142</v>
       </c>
@@ -3147,7 +3238,7 @@
         <v>0.15559999999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>143</v>
       </c>
@@ -3158,7 +3249,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>144</v>
       </c>
@@ -3169,7 +3260,7 @@
         <v>0.31619999999999998</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>145</v>
       </c>
@@ -3180,7 +3271,7 @@
         <v>0.32763999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>147</v>
       </c>
@@ -3191,7 +3282,7 @@
         <v>0.45304</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>146</v>
       </c>
@@ -3202,7 +3293,7 @@
         <v>0.48233999999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>157</v>
       </c>
@@ -3213,7 +3304,7 @@
         <v>0.21459</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>158</v>
       </c>
@@ -3224,7 +3315,7 @@
         <v>0.25752999999999998</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>159</v>
       </c>
@@ -3235,7 +3326,7 @@
         <v>0.49186000000000002</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>160</v>
       </c>
@@ -3246,7 +3337,7 @@
         <v>0.92889999999999995</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>161</v>
       </c>
@@ -3257,7 +3348,7 @@
         <v>0.37663999999999997</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>162</v>
       </c>
@@ -3268,7 +3359,7 @@
         <v>0.71209999999999996</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>164</v>
       </c>
@@ -3279,7 +3370,7 @@
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>165</v>
       </c>
@@ -3290,7 +3381,7 @@
         <v>7.6609999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>166</v>
       </c>
@@ -3301,7 +3392,7 @@
         <v>0.10367999999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>167</v>
       </c>
@@ -3312,7 +3403,7 @@
         <v>0.15343999999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>168</v>
       </c>
@@ -3323,7 +3414,7 @@
         <v>3.5360000000000003E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>169</v>
       </c>
@@ -3334,7 +3425,7 @@
         <v>4.2880000000000001E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>84</v>
       </c>
@@ -3345,7 +3436,7 @@
         <v>7.5230000000000005E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>85</v>
       </c>
@@ -3356,7 +3447,7 @@
         <v>7.4310000000000001E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>170</v>
       </c>
@@ -3367,7 +3458,7 @@
         <v>6.2710000000000002E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>171</v>
       </c>
@@ -3378,7 +3469,7 @@
         <v>8.43E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -3389,7 +3480,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>173</v>
       </c>
@@ -3400,7 +3491,7 @@
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>174</v>
       </c>
@@ -3411,7 +3502,7 @@
         <v>5.8099999999999999E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>175</v>
       </c>
@@ -3422,7 +3513,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>128</v>
       </c>
@@ -3433,7 +3524,7 @@
         <v>5.9799999999999999E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>129</v>
       </c>
@@ -3444,7 +3535,7 @@
         <v>7.8899999999999998E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>163</v>
       </c>
@@ -3455,7 +3546,7 @@
         <v>5.8400000000000001E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>176</v>
       </c>
@@ -3466,7 +3557,7 @@
         <v>7.0599999999999996E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>177</v>
       </c>
@@ -3477,7 +3568,7 @@
         <v>0.22586999999999999</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>178</v>
       </c>
@@ -3488,7 +3579,7 @@
         <v>0.254</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>179</v>
       </c>
@@ -3499,7 +3590,7 @@
         <v>8.9149999999999993E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>180</v>
       </c>
@@ -3510,7 +3601,7 @@
         <v>8.3659999999999998E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>181</v>
       </c>
@@ -3521,7 +3612,7 @@
         <v>7.7130000000000004E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>182</v>
       </c>
@@ -3532,7 +3623,7 @@
         <v>8.9370000000000005E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -3543,7 +3634,7 @@
         <v>6.3960000000000003E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>184</v>
       </c>
@@ -3554,7 +3645,7 @@
         <v>8.5180000000000006E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>185</v>
       </c>
@@ -3565,7 +3656,7 @@
         <v>7.3099999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>186</v>
       </c>
@@ -3576,7 +3667,7 @@
         <v>6.2640000000000001E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>187</v>
       </c>
@@ -3587,7 +3678,7 @@
         <v>6.4579999999999999E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>188</v>
       </c>
@@ -3598,7 +3689,7 @@
         <v>6.6769999999999996E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>189</v>
       </c>
@@ -3609,7 +3700,7 @@
         <v>2.452E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>190</v>
       </c>
@@ -3620,7 +3711,7 @@
         <v>2.93E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>191</v>
       </c>
@@ -3631,7 +3722,7 @@
         <v>8.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>192</v>
       </c>
@@ -3642,7 +3733,7 @@
         <v>8.4599999999999995E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>193</v>
       </c>
@@ -3653,7 +3744,7 @@
         <v>2.828E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>194</v>
       </c>
@@ -3664,7 +3755,7 @@
         <v>5.246E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>195</v>
       </c>
@@ -3675,7 +3766,7 @@
         <v>3.517E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>196</v>
       </c>
@@ -3686,7 +3777,7 @@
         <v>5.3830000000000003E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>197</v>
       </c>
@@ -3697,7 +3788,7 @@
         <v>6.4130000000000006E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>198</v>
       </c>
@@ -3708,7 +3799,7 @@
         <v>6.1170000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>76</v>
       </c>
@@ -3719,7 +3810,7 @@
         <v>6.0229999999999999E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>77</v>
       </c>
@@ -3730,7 +3821,7 @@
         <v>6.1469999999999997E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>132</v>
       </c>
@@ -3741,7 +3832,7 @@
         <v>0.41488999999999998</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>133</v>
       </c>
@@ -3752,7 +3843,7 @@
         <v>0.75600000000000001</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>199</v>
       </c>
@@ -3763,7 +3854,7 @@
         <v>5.5590000000000001E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>200</v>
       </c>
@@ -3774,7 +3865,7 @@
         <v>6.1019999999999998E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>201</v>
       </c>
@@ -3785,7 +3876,7 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>202</v>
       </c>
@@ -3796,7 +3887,7 @@
         <v>7.2040000000000007E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>98</v>
       </c>
@@ -3807,7 +3898,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>99</v>
       </c>
@@ -3818,7 +3909,7 @@
         <v>0.79190000000000005</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>203</v>
       </c>
@@ -3829,7 +3920,7 @@
         <v>0.13757</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>204</v>
       </c>
@@ -3840,7 +3931,7 @@
         <v>0.13672999999999999</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>205</v>
       </c>
@@ -3851,7 +3942,7 @@
         <v>6.5030000000000004E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>206</v>
       </c>
@@ -3862,7 +3953,7 @@
         <v>7.7950000000000005E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>207</v>
       </c>
@@ -3873,7 +3964,7 @@
         <v>8.6669999999999997E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>208</v>
       </c>
@@ -3884,7 +3975,7 @@
         <v>9.5200000000000007E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>116</v>
       </c>
@@ -3895,7 +3986,7 @@
         <v>3.2530000000000003E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>117</v>
       </c>
@@ -3906,7 +3997,7 @@
         <v>5.0250000000000003E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>209</v>
       </c>
@@ -3917,7 +4008,7 @@
         <v>6.4630000000000007E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>210</v>
       </c>
@@ -3928,7 +4019,7 @@
         <v>9.9790000000000004E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>211</v>
       </c>
@@ -3939,7 +4030,7 @@
         <v>4.4339999999999997E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>212</v>
       </c>
@@ -3950,7 +4041,7 @@
         <v>4.598E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>70</v>
       </c>
@@ -3961,7 +4052,7 @@
         <v>0.56067</v>
       </c>
     </row>
-    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>71</v>
       </c>
@@ -3972,7 +4063,7 @@
         <v>0.78349999999999997</v>
       </c>
     </row>
-    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>100</v>
       </c>
@@ -3983,7 +4074,7 @@
         <v>0.10165</v>
       </c>
     </row>
-    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>101</v>
       </c>
@@ -3994,7 +4085,7 @@
         <v>9.5829999999999999E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>213</v>
       </c>
@@ -4005,7 +4096,7 @@
         <v>5.457E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>214</v>
       </c>
@@ -4016,7 +4107,7 @@
         <v>9.4490000000000005E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>215</v>
       </c>
@@ -4027,7 +4118,7 @@
         <v>8.4070000000000006E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>216</v>
       </c>
@@ -4038,7 +4129,7 @@
         <v>0.10272000000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>217</v>
       </c>
@@ -4049,7 +4140,7 @@
         <v>1.8360000000000001E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>218</v>
       </c>
@@ -4060,7 +4151,7 @@
         <v>3.2649999999999998E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>219</v>
       </c>
@@ -4071,7 +4162,7 @@
         <v>7.8289999999999998E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>220</v>
       </c>
@@ -4082,7 +4173,7 @@
         <v>7.4079999999999993E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>221</v>
       </c>
@@ -4093,7 +4184,7 @@
         <v>3.2980000000000002E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>222</v>
       </c>
@@ -4104,7 +4195,7 @@
         <v>3.7440000000000001E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>223</v>
       </c>
@@ -4115,7 +4206,7 @@
         <v>0.11504</v>
       </c>
     </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>224</v>
       </c>
@@ -4126,7 +4217,7 @@
         <v>0.19739999999999999</v>
       </c>
     </row>
-    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>225</v>
       </c>
@@ -4137,7 +4228,7 @@
         <v>3.1620000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>226</v>
       </c>
@@ -4148,7 +4239,7 @@
         <v>6.0199999999999997E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>227</v>
       </c>
@@ -4159,7 +4250,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>228</v>
       </c>
@@ -4170,7 +4261,7 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>229</v>
       </c>
@@ -4181,7 +4272,7 @@
         <v>0.64200000000000002</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>230</v>
       </c>
@@ -4192,7 +4283,7 @@
         <v>0.77354999999999996</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>231</v>
       </c>
@@ -4203,7 +4294,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>232</v>
       </c>
@@ -4214,7 +4305,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>233</v>
       </c>
@@ -4225,7 +4316,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>234</v>
       </c>
@@ -4236,7 +4327,7 @@
         <v>0.6038</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>235</v>
       </c>
@@ -4247,7 +4338,7 @@
         <v>0.43169999999999997</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>236</v>
       </c>
@@ -4258,7 +4349,7 @@
         <v>0.43569999999999998</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>45</v>
       </c>
@@ -4269,7 +4360,7 @@
         <v>0.70094000000000001</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>46</v>
       </c>
@@ -4280,7 +4371,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>237</v>
       </c>
@@ -4291,7 +4382,7 @@
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>238</v>
       </c>
@@ -4302,7 +4393,7 @@
         <v>1.0084</v>
       </c>
     </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>239</v>
       </c>
@@ -4313,7 +4404,7 @@
         <v>0.27010000000000001</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>240</v>
       </c>
@@ -4324,7 +4415,7 @@
         <v>0.28236</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>4</v>
       </c>
@@ -4335,7 +4426,7 @@
         <v>0.43636000000000003</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>5</v>
       </c>
@@ -4346,7 +4437,7 @@
         <v>0.42949999999999999</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>43</v>
       </c>
@@ -4357,7 +4448,7 @@
         <v>0.15989999999999999</v>
       </c>
     </row>
-    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>44</v>
       </c>
@@ -4368,7 +4459,7 @@
         <v>0.16647000000000001</v>
       </c>
     </row>
-    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>241</v>
       </c>
@@ -4379,7 +4470,7 @@
         <v>0.6714</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>242</v>
       </c>
@@ -4390,7 +4481,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>51</v>
       </c>
@@ -4401,7 +4492,7 @@
         <v>0.17810999999999999</v>
       </c>
     </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>52</v>
       </c>
@@ -4412,7 +4503,7 @@
         <v>0.21096000000000001</v>
       </c>
     </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>7</v>
       </c>
@@ -4423,7 +4514,7 @@
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>8</v>
       </c>
@@ -4434,7 +4525,7 @@
         <v>0.79979999999999996</v>
       </c>
     </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>243</v>
       </c>
@@ -4445,7 +4536,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>244</v>
       </c>
@@ -4456,7 +4547,7 @@
         <v>0.48043999999999998</v>
       </c>
     </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>245</v>
       </c>
@@ -4467,7 +4558,7 @@
         <v>0.38150000000000001</v>
       </c>
     </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>246</v>
       </c>
@@ -4478,7 +4569,7 @@
         <v>0.43758999999999998</v>
       </c>
     </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>247</v>
       </c>
@@ -4489,7 +4580,7 @@
         <v>0.36170000000000002</v>
       </c>
     </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>248</v>
       </c>
@@ -4500,7 +4591,7 @@
         <v>0.39190999999999998</v>
       </c>
     </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>21</v>
       </c>
@@ -4511,7 +4602,7 @@
         <v>0.21812999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>22</v>
       </c>
@@ -4522,7 +4613,7 @@
         <v>0.27305000000000001</v>
       </c>
     </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>249</v>
       </c>
@@ -4533,7 +4624,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>250</v>
       </c>
@@ -4544,7 +4635,7 @@
         <v>0.55620000000000003</v>
       </c>
     </row>
-    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>251</v>
       </c>
@@ -4555,7 +4646,7 @@
         <v>0.40629999999999999</v>
       </c>
     </row>
-    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>252</v>
       </c>
@@ -4566,7 +4657,7 @@
         <v>0.45184000000000002</v>
       </c>
     </row>
-    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>257</v>
       </c>
@@ -4577,7 +4668,7 @@
         <v>0.58099999999999996</v>
       </c>
     </row>
-    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>258</v>
       </c>
@@ -4588,7 +4679,7 @@
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>9</v>
       </c>
@@ -4599,7 +4690,7 @@
         <v>0.14118</v>
       </c>
     </row>
-    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>10</v>
       </c>
@@ -4610,7 +4701,7 @@
         <v>0.29243000000000002</v>
       </c>
     </row>
-    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>239</v>
       </c>
@@ -4621,7 +4712,7 @@
         <v>0.29933999999999999</v>
       </c>
     </row>
-    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>240</v>
       </c>
@@ -4632,7 +4723,7 @@
         <v>0.33484999999999998</v>
       </c>
     </row>
-    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>255</v>
       </c>
@@ -4643,7 +4734,7 @@
         <v>0.1764</v>
       </c>
     </row>
-    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>256</v>
       </c>
@@ -4654,7 +4745,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>39</v>
       </c>
@@ -4665,7 +4756,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>40</v>
       </c>
@@ -4676,7 +4767,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>147</v>
       </c>
@@ -4687,7 +4778,7 @@
         <v>0.56899999999999995</v>
       </c>
     </row>
-    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>146</v>
       </c>
@@ -4698,7 +4789,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>4</v>
       </c>
@@ -4709,7 +4800,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>5</v>
       </c>
@@ -4720,7 +4811,7 @@
         <v>0.42393999999999998</v>
       </c>
     </row>
-    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>13</v>
       </c>
@@ -4731,7 +4822,7 @@
         <v>0.27007999999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>14</v>
       </c>
@@ -4742,7 +4833,7 @@
         <v>0.29982999999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>7</v>
       </c>
@@ -4753,7 +4844,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>8</v>
       </c>
@@ -4764,7 +4855,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>259</v>
       </c>
@@ -4775,7 +4866,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>260</v>
       </c>
@@ -4786,7 +4877,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>261</v>
       </c>
@@ -4797,7 +4888,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="309" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>262</v>
       </c>
@@ -4808,7 +4899,7 @@
         <v>0.74092999999999998</v>
       </c>
     </row>
-    <row r="310" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>263</v>
       </c>
@@ -4819,7 +4910,7 @@
         <v>0.31220999999999999</v>
       </c>
     </row>
-    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>264</v>
       </c>
@@ -4830,7 +4921,7 @@
         <v>0.57650000000000001</v>
       </c>
     </row>
-    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>251</v>
       </c>
@@ -4841,7 +4932,7 @@
         <v>0.54859999999999998</v>
       </c>
     </row>
-    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>252</v>
       </c>
@@ -4852,7 +4943,7 @@
         <v>0.66569999999999996</v>
       </c>
     </row>
-    <row r="314" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>265</v>
       </c>
@@ -4863,7 +4954,7 @@
         <v>0.65900000000000003</v>
       </c>
     </row>
-    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>265</v>
       </c>
@@ -5617,14 +5708,230 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F327">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F383"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>328</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>